<commit_message>
correct all the issue
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/HrmsTestData.xlsx
+++ b/src/test/resources/testdata/HrmsTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Project\eclipse-workspace\HrmsFramework\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{758D5D48-8C32-40B8-BACC-801C4C5E9518}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA80CF7-CDDD-4897-90AB-FC43BC7F7DA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20988" yWindow="324" windowWidth="17280" windowHeight="8964" xr2:uid="{CD3A54CB-C005-0E4A-932C-421D6A132F4C}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" xr2:uid="{CD3A54CB-C005-0E4A-932C-421D6A132F4C}"/>
   </bookViews>
   <sheets>
     <sheet name="EmployeeLoginCredentials" sheetId="1" r:id="rId1"/>
@@ -65,25 +65,25 @@
     <t>Akash</t>
   </si>
   <si>
-    <t>barhn4561</t>
-  </si>
-  <si>
     <t>Mayrw</t>
   </si>
   <si>
     <t>Kanshw</t>
   </si>
   <si>
-    <t>mayrw4561</t>
-  </si>
-  <si>
     <t>Akbar</t>
   </si>
   <si>
     <t>Tariq</t>
   </si>
   <si>
-    <t>Akbr4561</t>
+    <t>barhn45612</t>
+  </si>
+  <si>
+    <t>mayrw45612</t>
+  </si>
+  <si>
+    <t>Akbr45612</t>
   </si>
 </sst>
 </file>
@@ -460,7 +460,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.35"/>
@@ -494,7 +494,7 @@
         <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>4</v>
@@ -502,13 +502,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>4</v>
@@ -516,10 +516,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>18</v>

</xml_diff>